<commit_message>
Adding cross validation results
</commit_message>
<xml_diff>
--- a/cross_validation_results.xlsx
+++ b/cross_validation_results.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19E4EC6-3490-4AF9-BD81-FB2FC6F859B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30923F1F-7BCE-4573-BE84-E849A5B10EE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Model</t>
   </si>
@@ -65,6 +70,21 @@
   </si>
   <si>
     <t>Naïve-Nolags</t>
+  </si>
+  <si>
+    <t>1 Week</t>
+  </si>
+  <si>
+    <t>2 Week</t>
+  </si>
+  <si>
+    <t>3 Week</t>
+  </si>
+  <si>
+    <t>4 Week</t>
+  </si>
+  <si>
+    <t>5 Week</t>
   </si>
 </sst>
 </file>
@@ -363,7 +383,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -407,7 +427,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:f>Sheet1!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -717,7 +737,778 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Cummulative model</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" baseline="0"/>
+              <a:t> RMSE improvement over naive RMSE</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hibrid-LSTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$J$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 Week</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Week</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 Week</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 Week</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>17.403825655299897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83.695615000000089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206.02002063634018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>481.44450424835986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>615.23213925465006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-48D3-457E-9E70-9FAF236AEC89}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hibrid-LSTM-NoGT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$J$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 Week</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Week</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 Week</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 Week</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23.734720997489831</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-76.418610114179955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>222.83633688575992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>468.93697413726977</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>593.43617994679016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-48D3-457E-9E70-9FAF236AEC89}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pure-NN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$J$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 Week</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Week</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 Week</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 Week</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-150.27396041996008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.87961384301002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107.2863750546403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306.41680268046002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>523.6859855173002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-48D3-457E-9E70-9FAF236AEC89}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pure-NN-NoGT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$J$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 Week</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Week</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3 Week</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4 Week</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Week</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-131.54595374785004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-179.98634308908981</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-29.928252909239745</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>260.40340131421999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>472.97344792020021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-48D3-457E-9E70-9FAF236AEC89}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="764951064"/>
+        <c:axId val="764948112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="764951064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Week</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>s ahead</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764948112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="764948112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Naive RMSE - Model RMSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764951064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1260,6 +2051,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1293,6 +2600,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C56FCC8D-2713-46DE-9D98-57F714ED57CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1564,10 +2907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B12"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +2923,7 @@
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1599,8 +2942,26 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1619,8 +2980,31 @@
       <c r="F2" s="1">
         <v>2582.3927480795301</v>
       </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>B$6-B2</f>
+        <v>17.403825655299897</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:N2" si="0">C$6-C2</f>
+        <v>83.695615000000089</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>206.02002063634018</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>481.44450424835986</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>615.23213925465006</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1639,108 +3023,177 @@
       <c r="F3">
         <v>2604.18870738739</v>
       </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="1">B$6-B3</f>
+        <v>23.734720997489831</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K5" si="2">C$6-C3</f>
+        <v>-76.418610114179955</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L5" si="3">D$6-D3</f>
+        <v>222.83633688575992</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M5" si="4">E$6-E3</f>
+        <v>468.93697413726977</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N5" si="5">F$6-F3</f>
+        <v>593.43617994679016</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1319.18241180625</v>
+      </c>
+      <c r="C4">
+        <v>1896.9423021569901</v>
+      </c>
+      <c r="D4">
+        <v>2289.3991035816998</v>
+      </c>
+      <c r="E4">
+        <v>2569.2783534129999</v>
+      </c>
+      <c r="F4">
+        <v>2673.9389018168799</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>-150.27396041996008</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>15.87961384301002</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>107.2863750546403</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>306.41680268046002</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>523.6859855173002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1300.45440513414</v>
+      </c>
+      <c r="C5">
+        <v>2092.8082590890899</v>
+      </c>
+      <c r="D5">
+        <v>2426.6137315455799</v>
+      </c>
+      <c r="E5">
+        <v>2615.2917547792399</v>
+      </c>
+      <c r="F5">
+        <v>2724.6514394139799</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>-131.54595374785004</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>-179.98634308908981</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>-29.928252909239745</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>260.40340131421999</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>472.97344792020021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1168.9084513862899</v>
+      </c>
+      <c r="C6">
+        <v>1912.8219160000001</v>
+      </c>
+      <c r="D6">
+        <v>2396.6854786363401</v>
+      </c>
+      <c r="E6">
+        <v>2875.6951560934599</v>
+      </c>
+      <c r="F6">
+        <v>3197.6248873341801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <v>4027.4966562488898</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>4093.37170352669</v>
       </c>
-      <c r="D4">
+      <c r="D7">
         <v>4041.6698507422102</v>
       </c>
-      <c r="E4">
+      <c r="E7">
         <v>3637.4483825352399</v>
       </c>
-      <c r="F4">
+      <c r="F7">
         <v>3509.8739492466698</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>3828.06348592515</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>3929.7425686991601</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <v>3919.3122609786201</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>3536.3682195781698</v>
       </c>
-      <c r="F5">
+      <c r="F8">
         <v>3565.9480272239498</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>1319.18241180625</v>
-      </c>
-      <c r="C6">
-        <v>1896.9423021569901</v>
-      </c>
-      <c r="D6">
-        <v>2289.3991035816998</v>
-      </c>
-      <c r="E6">
-        <v>2569.2783534129999</v>
-      </c>
-      <c r="F6">
-        <v>2673.9389018168799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>1300.45440513414</v>
-      </c>
-      <c r="C7">
-        <v>2092.8082590890899</v>
-      </c>
-      <c r="D7">
-        <v>2426.6137315455799</v>
-      </c>
-      <c r="E7">
-        <v>2615.2917547792399</v>
-      </c>
-      <c r="F7">
-        <v>2724.6514394139799</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1168.9084513862899</v>
-      </c>
-      <c r="C8">
-        <v>1912.8219160000001</v>
-      </c>
-      <c r="D8">
-        <v>2396.6854786363401</v>
-      </c>
-      <c r="E8">
-        <v>2875.6951560934599</v>
-      </c>
-      <c r="F8">
-        <v>3197.6248873341801</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1748,7 +3201,7 @@
         <v>1535.29276783816</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>

</xml_diff>